<commit_message>
Updated Consolidated error messages for IDA
</commit_message>
<xml_diff>
--- a/docs/requirements/Requirements Detailing References/ID-Authentication/Sprint 9/Consolidated error messages V2.1.xlsx
+++ b/docs/requirements/Requirements Detailing References/ID-Authentication/Sprint 9/Consolidated error messages V2.1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIPRequirementsGithub\docs\requirements\Requirements Detailing References\ID-Authentication\Sprint 9\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIP\Project\User stories\Authenticatoin_New Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7AE3939F-2B94-4268-8FA2-7032875923D3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{738609DD-A2F0-42E7-96D5-DA03AA193729}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7125" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">IDA!$A$1:$F$67</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">IDA!$A$1:$F$69</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -137,7 +137,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="307">
   <si>
     <t>IDA-MLC-003</t>
   </si>
@@ -1183,6 +1183,15 @@
   </si>
   <si>
     <t>"HMAC Validation failed"</t>
+  </si>
+  <si>
+    <t>IDA-OTA-010</t>
+  </si>
+  <si>
+    <t>No OTP Channel is provided in the input</t>
+  </si>
+  <si>
+    <t>"OTP Notification Channel not provided."</t>
   </si>
 </sst>
 </file>
@@ -1348,7 +1357,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1399,6 +1408,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1406,7 +1426,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1467,6 +1487,9 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1814,10 +1837,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H76"/>
+  <dimension ref="A1:K76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68:F68"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.7109375" defaultRowHeight="28.5" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1937,7 +1960,7 @@
       </c>
       <c r="G5" s="12"/>
     </row>
-    <row r="6" spans="1:7" ht="63" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>5</v>
       </c>
@@ -1958,7 +1981,7 @@
       </c>
       <c r="G6" s="12"/>
     </row>
-    <row r="7" spans="1:7" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>6</v>
       </c>
@@ -1979,7 +2002,7 @@
       </c>
       <c r="G7" s="15"/>
     </row>
-    <row r="8" spans="1:7" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>7</v>
       </c>
@@ -1996,7 +2019,7 @@
       </c>
       <c r="G8" s="12"/>
     </row>
-    <row r="9" spans="1:7" ht="47.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>8</v>
       </c>
@@ -2013,7 +2036,7 @@
       </c>
       <c r="G9" s="12"/>
     </row>
-    <row r="10" spans="1:7" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -2034,7 +2057,7 @@
       </c>
       <c r="G10" s="12"/>
     </row>
-    <row r="11" spans="1:7" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -2055,7 +2078,7 @@
       </c>
       <c r="G11" s="12"/>
     </row>
-    <row r="12" spans="1:7" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -2487,7 +2510,7 @@
       </c>
       <c r="G34" s="12"/>
     </row>
-    <row r="35" spans="1:7" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10">
         <v>34</v>
       </c>
@@ -2540,7 +2563,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="10">
         <v>37</v>
       </c>
@@ -2557,7 +2580,7 @@
       </c>
       <c r="G38" s="12"/>
     </row>
-    <row r="39" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="10">
         <v>38</v>
       </c>
@@ -2574,7 +2597,7 @@
       </c>
       <c r="G39" s="12"/>
     </row>
-    <row r="40" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="47.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10">
         <v>39</v>
       </c>
@@ -2591,7 +2614,7 @@
       </c>
       <c r="G40" s="12"/>
     </row>
-    <row r="41" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="10">
         <v>40</v>
       </c>
@@ -2640,7 +2663,7 @@
       <c r="F43" s="12"/>
       <c r="G43" s="12"/>
     </row>
-    <row r="44" spans="1:7" ht="47.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A44" s="10">
         <v>43</v>
       </c>
@@ -2657,7 +2680,7 @@
       </c>
       <c r="G44" s="12"/>
     </row>
-    <row r="45" spans="1:7" ht="63" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="63" x14ac:dyDescent="0.25">
       <c r="A45" s="10">
         <v>44</v>
       </c>
@@ -2822,7 +2845,7 @@
       </c>
       <c r="G53" s="12"/>
     </row>
-    <row r="54" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="10">
         <v>53</v>
       </c>
@@ -2841,7 +2864,7 @@
       </c>
       <c r="G54" s="12"/>
     </row>
-    <row r="55" spans="1:7" s="8" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" s="8" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="10">
         <v>54</v>
       </c>
@@ -2862,7 +2885,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="63" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="63" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="10">
         <v>55</v>
       </c>
@@ -2879,7 +2902,7 @@
       </c>
       <c r="G56" s="12"/>
     </row>
-    <row r="57" spans="1:7" ht="63" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="63" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="10">
         <v>56</v>
       </c>
@@ -2896,7 +2919,7 @@
       </c>
       <c r="G57" s="12"/>
     </row>
-    <row r="58" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="47.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="10">
         <v>57</v>
       </c>
@@ -2913,7 +2936,7 @@
       </c>
       <c r="G58" s="12"/>
     </row>
-    <row r="59" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="10">
         <v>58</v>
       </c>
@@ -2930,7 +2953,7 @@
       </c>
       <c r="G59" s="12"/>
     </row>
-    <row r="60" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="10">
         <v>59</v>
       </c>
@@ -2947,7 +2970,7 @@
       </c>
       <c r="G60" s="12"/>
     </row>
-    <row r="61" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="10">
         <v>60</v>
       </c>
@@ -2964,7 +2987,7 @@
       </c>
       <c r="G61" s="12"/>
     </row>
-    <row r="62" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="10">
         <v>61</v>
       </c>
@@ -2981,7 +3004,7 @@
       </c>
       <c r="G62" s="12"/>
     </row>
-    <row r="63" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="10">
         <v>62</v>
       </c>
@@ -3015,7 +3038,7 @@
       </c>
       <c r="G64" s="12"/>
     </row>
-    <row r="65" spans="1:7" ht="28.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" ht="28.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="19">
         <v>64</v>
       </c>
@@ -3032,7 +3055,7 @@
       </c>
       <c r="G65" s="7"/>
     </row>
-    <row r="66" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="10">
         <v>63</v>
       </c>
@@ -3049,7 +3072,7 @@
       </c>
       <c r="G66" s="12"/>
     </row>
-    <row r="67" spans="1:7" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" ht="94.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="10">
         <v>64</v>
       </c>
@@ -3066,7 +3089,7 @@
       </c>
       <c r="G67" s="12"/>
     </row>
-    <row r="68" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="10">
         <v>65</v>
       </c>
@@ -3083,32 +3106,48 @@
       </c>
       <c r="G68" s="12"/>
     </row>
-    <row r="71" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="25">
+        <v>66</v>
+      </c>
+      <c r="B69" s="11" t="s">
+        <v>305</v>
+      </c>
+      <c r="C69" s="16" t="s">
+        <v>306</v>
+      </c>
+      <c r="D69" s="12"/>
+      <c r="E69" s="11"/>
+      <c r="F69" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="G69" s="16"/>
+      <c r="H69" s="12"/>
+      <c r="I69" s="11"/>
+      <c r="J69" s="12"/>
+      <c r="K69" s="11"/>
+    </row>
+    <row r="71" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
     </row>
-    <row r="76" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C76" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F67" xr:uid="{00000000-0009-0000-0000-000000000000}">
+  <autoFilter ref="A1:F69" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="5">
       <filters>
-        <filter val="IDA-MPA-001"/>
-        <filter val="IDA-MPA-002"/>
-        <filter val="IDA-MPA-003"/>
-        <filter val="IDA-MPA-004"/>
-        <filter val="IDA-MPA-005"/>
-        <filter val="IDA-MPA-006"/>
-        <filter val="IDA-MPA-007"/>
-        <filter val="IDA-MPA-008"/>
-        <filter val="IDA-MPA-009"/>
-        <filter val="IDA-MPA-010"/>
-        <filter val="IDA-MPA-011"/>
-        <filter val="IDA-MPA-012"/>
-        <filter val="IDA-MPA-013"/>
-        <filter val="IDA-MPA-014"/>
-        <filter val="IDA-MPA-015"/>
+        <filter val="IDA-OTA-001"/>
+        <filter val="IDA-OTA-002"/>
+        <filter val="IDA-OTA-003"/>
+        <filter val="IDA-OTA-004"/>
+        <filter val="IDA-OTA-005"/>
+        <filter val="IDA-OTA-006"/>
+        <filter val="IDA-OTA-007"/>
+        <filter val="IDA-OTA-008"/>
+        <filter val="IDA-OTA-009"/>
+        <filter val="IDA-OTA-010"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>